<commit_message>
Added canonical url support, fixed sitemap controller.
</commit_message>
<xml_diff>
--- a/src/WebMarket/WebMarket/App_Data/Products.xlsx
+++ b/src/WebMarket/WebMarket/App_Data/Products.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="avr" sheetId="1" r:id="rId1"/>
@@ -5711,7 +5711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN268"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A257" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
@@ -31617,7 +31617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>

</xml_diff>